<commit_message>
Minor corrections on Inductor Calculations are made - Unnecessary Files are Removed
</commit_message>
<xml_diff>
--- a/Component Selection for Cuk and Buck-Boost Converter.xlsx
+++ b/Component Selection for Cuk and Buck-Boost Converter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\ee464-HW1\Q2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\ee464-HW1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C890588-8BC7-477C-86CE-41B17CEBDD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECBA7B0-88AF-43DE-9D7E-5D2B75375520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Component</t>
   </si>
@@ -156,7 +156,16 @@
     <t xml:space="preserve">Diode </t>
   </si>
   <si>
-    <t>$10.78</t>
+    <t>PQ108081-471MHF</t>
+  </si>
+  <si>
+    <t>4.5A</t>
+  </si>
+  <si>
+    <t>$6.9000</t>
+  </si>
+  <si>
+    <t>$8.52</t>
   </si>
 </sst>
 </file>
@@ -219,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,8 +260,14 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -301,6 +316,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -310,7 +353,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
@@ -318,6 +361,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -606,7 +658,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +676,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,23 +696,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="9">
         <v>1</v>
       </c>
     </row>
@@ -729,7 +781,7 @@
         <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>